<commit_message>
add get/update grades routes
</commit_message>
<xml_diff>
--- a/static/temp/groups.xlsx
+++ b/static/temp/groups.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chunai\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58789D3E-F72E-4A0B-871C-E0F23733FDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Лист2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Лист3" sheetId="3" r:id="rId6"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="Q53o0pUy/+sJprWfhY01uewXBdJ1Ds/heqZqzuOp3LI="/>
@@ -18,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="111">
   <si>
     <t>N</t>
   </si>
@@ -342,26 +351,35 @@
   </si>
   <si>
     <t>Беспилотная робототехника</t>
+  </si>
+  <si>
+    <t>201-322</t>
+  </si>
+  <si>
+    <t>201-321</t>
+  </si>
+  <si>
+    <t>Академический учебный план 000019339 от 31.01.2024 11:51:06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF333300"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -371,7 +389,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -381,7 +399,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF993300"/>
@@ -395,46 +419,42 @@
       <bottom style="thin">
         <color rgb="FF993300"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -624,25 +644,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="8.71"/>
-    <col customWidth="1" min="3" max="3" width="55.14"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,9 +699,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
@@ -712,9 +734,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>21</v>
@@ -747,9 +769,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>22</v>
@@ -782,9 +804,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>28</v>
@@ -817,9 +839,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>31</v>
@@ -852,9 +874,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>32</v>
@@ -887,9 +909,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>35</v>
@@ -922,9 +944,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>36</v>
@@ -957,9 +979,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>39</v>
@@ -992,9 +1014,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>40</v>
@@ -1027,9 +1049,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>43</v>
@@ -1062,9 +1084,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>44</v>
@@ -1097,9 +1119,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>49</v>
@@ -1132,9 +1154,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>50</v>
@@ -1167,9 +1189,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11">
       <c r="A16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>51</v>
@@ -1202,9 +1224,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11">
       <c r="A17" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>52</v>
@@ -1237,9 +1259,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:11">
       <c r="A18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>53</v>
@@ -1272,9 +1294,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:11">
       <c r="A19" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>54</v>
@@ -1307,9 +1329,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:11">
       <c r="A20" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>55</v>
@@ -1342,9 +1364,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>60</v>
@@ -1377,9 +1399,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>61</v>
@@ -1412,9 +1434,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>65</v>
@@ -1447,9 +1469,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>66</v>
@@ -1482,9 +1504,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>71</v>
@@ -1517,9 +1539,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>72</v>
@@ -1552,9 +1574,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="A27" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>74</v>
@@ -1587,9 +1609,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
       <c r="A28" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>77</v>
@@ -1622,9 +1644,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1">
       <c r="A29" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>79</v>
@@ -1657,9 +1679,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1">
       <c r="A30" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>81</v>
@@ -1692,9 +1714,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1">
       <c r="A31" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>87</v>
@@ -1727,9 +1749,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1">
       <c r="A32" s="2">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>88</v>
@@ -1762,9 +1784,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1">
       <c r="A33" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>92</v>
@@ -1797,9 +1819,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:11" ht="15.75" customHeight="1">
       <c r="A34" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>93</v>
@@ -1832,9 +1854,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:11" ht="15.75" customHeight="1">
       <c r="A35" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>97</v>
@@ -1867,9 +1889,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:11" ht="15.75" customHeight="1">
       <c r="A36" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>98</v>
@@ -1902,9 +1924,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:11" ht="15.75" customHeight="1">
       <c r="A37" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>102</v>
@@ -1937,9 +1959,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:11" ht="15.75" customHeight="1">
       <c r="A38" s="2">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>103</v>
@@ -1972,16 +1994,84 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2935,24 +3025,20 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A21:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -3936,24 +4022,20 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A21:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -4937,9 +5019,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>